<commit_message>
aggiornati risultati su excel
</commit_message>
<xml_diff>
--- a/results/PythonExport.xlsx
+++ b/results/PythonExport.xlsx
@@ -112,24 +112,24 @@
     <t>Avviata anteprima tentativo quiz</t>
   </si>
   <si>
+    <t>Aggiornato gruppo</t>
+  </si>
+  <si>
     <t>Eliminato evento di calendario</t>
   </si>
   <si>
-    <t>Aggiornato gruppo</t>
-  </si>
-  <si>
     <t>Visualizzato report log</t>
   </si>
   <si>
+    <t>Inserito intervento nel forum</t>
+  </si>
+  <si>
+    <t>Creato gruppo</t>
+  </si>
+  <si>
     <t>Creata discussione</t>
   </si>
   <si>
-    <t>Creato gruppo</t>
-  </si>
-  <si>
-    <t>Inserito intervento nel forum</t>
-  </si>
-  <si>
     <t>Visualizzato report attività del corso</t>
   </si>
   <si>
@@ -172,19 +172,19 @@
     <t>Creata istanza metodo d'iscrizione</t>
   </si>
   <si>
+    <t>Aggiornata istanza metodo d'iscrizione</t>
+  </si>
+  <si>
     <t>Creato corso</t>
   </si>
   <si>
     <t>Ripristinato corso</t>
   </si>
   <si>
-    <t>Aggiornata istanza metodo d'iscrizione</t>
+    <t>Revocato ruolo</t>
   </si>
   <si>
     <t>Disiscritto utente dal corso</t>
-  </si>
-  <si>
-    <t>Revocato ruolo</t>
   </si>
   <si>
     <t>Visualizzato registro valutatore</t>

</xml_diff>